<commit_message>
add function compare content
</commit_message>
<xml_diff>
--- a/0.Python/Basic_func/input/Book1.xlsx
+++ b/0.Python/Basic_func/input/Book1.xlsx
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -201,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,13 +582,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="15.875" customWidth="1" min="12" max="12"/>
+    <col width="17.625" customWidth="1" min="14" max="14"/>
+  </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
@@ -651,6 +658,11 @@
       <c r="M1" t="inlineStr">
         <is>
           <t>Check Consistency</t>
+        </is>
+      </c>
+      <c r="N1" s="13" t="inlineStr">
+        <is>
+          <t>TS_TestDesciption</t>
         </is>
       </c>
     </row>
@@ -720,6 +732,23 @@
           <t>OK</t>
         </is>
       </c>
+      <c r="N2" s="12" t="inlineStr">
+        <is>
+          <t>**Precondition: 
+	1. Flashing of “XCPACTDEV” file*
+	(ex.
+	a.	5G3: FL_3WA907541F_&lt;Release&gt;_XCPACTDEV_XXXX_E.pdx
+	b.	5G5: FL_3WA907670F_&lt;Release&gt;_XCPACTDEV_XXXX_E.pdx)
+	2. SFD: available
+	3. Deactive all PDA group before check for each case
+CASE 1:
+Set: "WriteDataByIdentifierRequest[Group 3 Xcp].bit 5" == 'Enabled'
+Check: the Sensor(Hella)Development Messages is sent on VCAN-Bus
+CASE 2:
+Set: "WriteDataByIdentifierRequest[Group 3 Xcp].bit 5" &lt;&gt; 'Enabled'
+Check: Sending Sensor(Hella)Development Messages shall be stopped on VCAN.</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="2" t="n">
@@ -769,6 +798,7 @@
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="2" t="n">
@@ -820,6 +850,7 @@
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="2" t="n">
@@ -871,6 +902,7 @@
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="2" t="n">
@@ -922,6 +954,7 @@
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="2" t="n">
@@ -973,6 +1006,7 @@
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="2" t="n">
@@ -1020,6 +1054,7 @@
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="2" t="n">
@@ -1091,6 +1126,7 @@
           <t>OK</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="2" t="n">
@@ -1138,6 +1174,7 @@
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="2" t="n">
@@ -1189,6 +1226,7 @@
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="2" t="n">
@@ -1236,6 +1274,7 @@
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="2" t="n">
@@ -1283,6 +1322,7 @@
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="2" t="n">
@@ -1330,12 +1370,13 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;8&amp;K808080 INTERNAL &amp; PARTNERS&amp;1#_x000d_&amp;"Arial"&amp;11&amp;K000000&amp;"Calibri"&amp;1 &amp;K808080 INTERNAL &amp; PARTNERS#_x000d_</oddHeader>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;8&amp;K808080 INTERNAL &amp; PARTNERS&amp;1#_x000d_&amp;"Arial"&amp;11&amp;K000000&amp;"Arial"&amp;11&amp;K000000&amp;"Calibri"&amp;1 &amp;K808080 INTERNAL &amp; PARTNERS#_x000d_</oddHeader>
     <oddFooter>&amp;R&amp;"Calibri"&amp;2 &amp;KFFFFFF_x000d_# 5acXjzUk_x000d_&amp;1#&amp;"Calibri"&amp;2 &amp;KFFFFFF 5acXjzUk</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>